<commit_message>
Ajout de @CompileStatic terminé et amélioration
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>ZZ.XXX.001.LEC</t>
-  </si>
-  <si>
-    <t>RO.FOU.001.CRE.01</t>
   </si>
 </sst>
 </file>
@@ -477,7 +474,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A8:A9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -500,25 +497,31 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
@@ -527,7 +530,9 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
@@ -536,6 +541,9 @@
       </c>
     </row>
     <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
retour arriere sur les modif écrans
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -474,7 +474,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -497,20 +497,20 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
+      <c r="A4" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
@@ -520,9 +520,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
@@ -531,9 +529,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="A6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
@@ -542,9 +538,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
@@ -553,9 +547,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
ajout  RESULTAT DES TESTS dans TO DO LIST
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>ZZ.XXX.001.LEC</t>
+  </si>
+  <si>
+    <t>RO.FOU.001.SUP.01</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -497,38 +500,25 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
+      <c r="A7" s="2"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2"/>
@@ -561,7 +551,7 @@
   <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
update RT.ART --> REC SUP LEC OK --> MAJ en cours
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -116,7 +116,10 @@
     <t>ZZ.XXX.001.LEC</t>
   </si>
   <si>
-    <t>RO.FOU.001.SUP.01</t>
+    <t>RT.ART</t>
+  </si>
+  <si>
+    <t>RT.ART.001.MAJ</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B8" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -505,14 +508,8 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2"/>
@@ -551,7 +548,7 @@
   <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -644,6 +641,9 @@
       <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="2" t="s">

</xml_diff>

<commit_message>
Supression de CHECKALLDATAS, ajout du ctrl groupé des TBD dans les log
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -119,7 +119,10 @@
     <t>RT.ART</t>
   </si>
   <si>
-    <t>RT.ART.001.CRE</t>
+    <t>RT.MAT.001.REC</t>
+  </si>
+  <si>
+    <t>RT.MAT.001.SUP</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -509,6 +512,11 @@
     <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4">

</xml_diff>

<commit_message>
Correction + debut RT.MAT
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>RT.MAT.001.REC</t>
-  </si>
-  <si>
-    <t>RT.MAT.001.SUP</t>
   </si>
 </sst>
 </file>
@@ -483,7 +480,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -512,11 +509,6 @@
     <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4">

</xml_diff>

<commit_message>
update + AD.DEP --> en cours
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -119,7 +119,7 @@
     <t>RT.ART</t>
   </si>
   <si>
-    <t>RT.MAT.001.REC</t>
+    <t>AD.DEP.001.FON.01</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -507,7 +507,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -545,7 +545,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F15"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -636,57 +636,65 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
-      <c r="B15" t="s">
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update + test sigcheck
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -480,7 +480,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -503,19 +503,48 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2"/>
@@ -545,10 +574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F17"/>
+  <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -649,9 +678,6 @@
       <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="2" t="s">
@@ -671,7 +697,7 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>30</v>
@@ -679,7 +705,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>31</v>
@@ -687,14 +713,24 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update + add sql distant + restore
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>RO.ORG</t>
-  </si>
-  <si>
-    <t>RO.ORG.001.REC</t>
   </si>
 </sst>
 </file>
@@ -489,7 +486,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -512,31 +509,48 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="D11" s="2"/>
@@ -551,7 +565,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B11" sqref="B11:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Global Update et correction addTraceBEGIN et END
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -483,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -509,16 +509,49 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gros update refonte code
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -168,6 +168,30 @@
   </si>
   <si>
     <t>RT.MAT.001.CRE.04</t>
+  </si>
+  <si>
+    <t>RO.ACT.001</t>
+  </si>
+  <si>
+    <t>RO.ACT.003</t>
+  </si>
+  <si>
+    <t>RO.ACT.005</t>
+  </si>
+  <si>
+    <t>RO.FOU.001</t>
+  </si>
+  <si>
+    <t>MP.CPT.001</t>
+  </si>
+  <si>
+    <t>RT.ART.001</t>
+  </si>
+  <si>
+    <t>RT.MAT.001</t>
+  </si>
+  <si>
+    <t>RO.ORG.001</t>
   </si>
 </sst>
 </file>
@@ -525,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A11"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -537,9 +561,7 @@
     <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -560,28 +582,62 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -591,10 +647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -815,10 +871,46 @@
       <c r="C22" t="s">
         <v>50</v>
       </c>
+      <c r="F22" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="23" spans="2:6">
       <c r="C23" t="s">
         <v>19</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="F24" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="F25" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="F26" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="F27" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="F29" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grosse refonte renommage des package et class
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -552,7 +552,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -576,66 +576,104 @@
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>57</v>
       </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>58</v>
       </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -650,7 +688,7 @@
   <dimension ref="B2:F29"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B14"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Gestion des input RADIO
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -600,7 +600,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+      <selection activeCell="B15" sqref="B15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -623,7 +623,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>60</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="D3" s="2" t="s">
@@ -648,6 +648,9 @@
       </c>
     </row>
     <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
@@ -659,6 +662,9 @@
       </c>
     </row>
     <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
@@ -667,6 +673,9 @@
       </c>
     </row>
     <row r="6" spans="1:8">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
@@ -675,6 +684,9 @@
       </c>
     </row>
     <row r="7" spans="1:8">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
@@ -683,6 +695,9 @@
       </c>
     </row>
     <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
@@ -691,6 +706,9 @@
       </c>
     </row>
     <row r="9" spans="1:8">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
@@ -699,6 +717,9 @@
       </c>
     </row>
     <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
@@ -707,6 +728,9 @@
       </c>
     </row>
     <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
       <c r="D11" t="s">
         <v>35</v>
       </c>
@@ -715,6 +739,9 @@
       </c>
     </row>
     <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
       <c r="D12" t="s">
         <v>36</v>
       </c>
@@ -723,6 +750,9 @@
       </c>
     </row>
     <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
       <c r="D13" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Version avec stepID numeric dans les STEP
Commit avant changement de stratégie pour le stepID
Fonctionne mais tous les STEP ne sont pas maj avec les numéro de STEP
dans les cas de test, ce qui a été fait c'est 
AD 
MP 
RO.ACT.001
RO.ACT.003HAB.SRA
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>TR.BTR.001.LEC</t>
+  </si>
+  <si>
+    <t>MP.CPT.001.CRE</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -623,7 +626,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>60</v>
@@ -633,8 +636,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>19</v>
       </c>
       <c r="B3" s="2"/>
       <c r="D3" s="2" t="s">
@@ -648,9 +651,6 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
@@ -662,9 +662,6 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
@@ -673,9 +670,6 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
@@ -717,6 +711,9 @@
       <c r="F10" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="H10" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="D11" t="s">
@@ -735,6 +732,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
+      <c r="B13" s="2"/>
       <c r="D13" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Update avant repise correction JDD
Correction générale suite à test LOT1A
Ajout de Macro STEP pour les cas de test SUP et REC
</commit_message>
<xml_diff>
--- a/TNR/_TNRSequencer.xlsx
+++ b/TNR/_TNRSequencer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>CAS_DE_TEST</t>
   </si>
@@ -603,7 +603,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B12" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -626,7 +626,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>60</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="D3" s="2" t="s">
@@ -651,8 +651,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>19</v>
+      <c r="A4" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
@@ -665,6 +665,9 @@
       </c>
     </row>
     <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
@@ -673,6 +676,9 @@
       </c>
     </row>
     <row r="6" spans="1:8">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
@@ -681,6 +687,9 @@
       </c>
     </row>
     <row r="7" spans="1:8">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
@@ -689,6 +698,9 @@
       </c>
     </row>
     <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
@@ -700,6 +712,9 @@
       </c>
     </row>
     <row r="9" spans="1:8">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
@@ -708,6 +723,9 @@
       </c>
     </row>
     <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
@@ -719,6 +737,9 @@
       </c>
     </row>
     <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
       <c r="D11" t="s">
         <v>35</v>
       </c>
@@ -727,6 +748,9 @@
       </c>
     </row>
     <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
       <c r="D12" t="s">
         <v>36</v>
       </c>
@@ -735,6 +759,9 @@
       </c>
     </row>
     <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="D13" t="s">
         <v>59</v>

</xml_diff>